<commit_message>
add amazon-google idf notebook
</commit_message>
<xml_diff>
--- a/notebooks/amazon-google-results.xlsx
+++ b/notebooks/amazon-google-results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="41020" yWindow="-10760" windowWidth="28040" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="41040" yWindow="-10740" windowWidth="30900" windowHeight="17620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="48">
   <si>
     <t>Vocabulary</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Average, IDF, Bi-LSTM</t>
   </si>
   <si>
-    <t>Cosine, Inverse_l1, Inverse_l2</t>
-  </si>
-  <si>
     <t>base_1</t>
   </si>
   <si>
@@ -141,6 +138,36 @@
   </si>
   <si>
     <t>F-Score</t>
+  </si>
+  <si>
+    <t>base_1t_num</t>
+  </si>
+  <si>
+    <t>base_1t_num_null</t>
+  </si>
+  <si>
+    <t>base_1t_num_null_allsim</t>
+  </si>
+  <si>
+    <t>Cosine, Inverse_l1</t>
+  </si>
+  <si>
+    <t>(32, 16)</t>
+  </si>
+  <si>
+    <t>LSTM nodes / Dropout</t>
+  </si>
+  <si>
+    <t>25 / 0 / 0</t>
+  </si>
+  <si>
+    <t>Dropout</t>
+  </si>
+  <si>
+    <t>base_2t_separate</t>
+  </si>
+  <si>
+    <t>Bi-LSTM (not shared)</t>
   </si>
 </sst>
 </file>
@@ -189,8 +216,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -239,7 +282,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -262,6 +305,14 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -284,6 +335,14 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -559,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -574,10 +633,10 @@
     <col min="5" max="5" width="27.83203125" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -597,21 +656,27 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>25</v>
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
       </c>
       <c r="J1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
         <v>36</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -631,22 +696,22 @@
       <c r="G2" t="b">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2">
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2">
         <v>0.78</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>0.56999999999999995</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>0.66</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -666,13 +731,22 @@
       <c r="G3" t="b">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3">
+        <v>0.78</v>
+      </c>
+      <c r="M3">
+        <v>0.68</v>
+      </c>
+      <c r="N3">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -693,12 +767,27 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4">
+        <v>0.5</v>
+      </c>
+      <c r="L4">
+        <v>0.73</v>
+      </c>
+      <c r="M4">
+        <v>0.88</v>
+      </c>
+      <c r="N4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -718,13 +807,13 @@
       <c r="G5" t="b">
         <v>0</v>
       </c>
-      <c r="H5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -736,7 +825,7 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -744,22 +833,22 @@
       <c r="G7" t="b">
         <v>0</v>
       </c>
-      <c r="H7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7">
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7">
         <v>0.79</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>0.65</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>0.71</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -771,7 +860,7 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -779,13 +868,13 @@
       <c r="G8" t="b">
         <v>0</v>
       </c>
-      <c r="H8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -797,7 +886,7 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -805,13 +894,13 @@
       <c r="G9" t="b">
         <v>0</v>
       </c>
-      <c r="H9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -823,7 +912,7 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -831,13 +920,13 @@
       <c r="G10" t="b">
         <v>0</v>
       </c>
-      <c r="H10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -857,13 +946,22 @@
       <c r="G12" t="b">
         <v>0</v>
       </c>
-      <c r="H12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12">
+        <v>0.9</v>
+      </c>
+      <c r="M12">
+        <v>0.84</v>
+      </c>
+      <c r="N12">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -883,119 +981,110 @@
       <c r="G13" t="b">
         <v>0</v>
       </c>
-      <c r="H13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="I13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16">
+        <v>0.83</v>
+      </c>
+      <c r="M16">
+        <v>0.53</v>
+      </c>
+      <c r="N16">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="C15" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
         <v>7</v>
       </c>
-      <c r="E15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15">
-        <v>0.83</v>
-      </c>
-      <c r="K15">
-        <v>0.53</v>
-      </c>
-      <c r="L15">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18">
-        <v>0.7</v>
-      </c>
-      <c r="K18">
-        <v>0.76</v>
-      </c>
-      <c r="L18">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" t="s">
-        <v>9</v>
-      </c>
       <c r="E19" t="s">
         <v>8</v>
       </c>
@@ -1005,19 +1094,28 @@
       <c r="G19" t="b">
         <v>0</v>
       </c>
-      <c r="H19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>25</v>
+      </c>
+      <c r="L19">
+        <v>0.88</v>
+      </c>
+      <c r="M19">
+        <v>0.9</v>
+      </c>
+      <c r="N19">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -1026,143 +1124,293 @@
         <v>8</v>
       </c>
       <c r="F20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
+        <v>25</v>
+      </c>
+      <c r="L20">
+        <v>0.87</v>
+      </c>
+      <c r="M20">
+        <v>0.92</v>
+      </c>
+      <c r="N20">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>25</v>
+      </c>
+      <c r="L21">
+        <v>0.89</v>
+      </c>
+      <c r="M21">
+        <v>0.91</v>
+      </c>
+      <c r="N21">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23">
+        <v>0.7</v>
+      </c>
+      <c r="M23">
+        <v>0.76</v>
+      </c>
+      <c r="N23">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>25</v>
+      </c>
+      <c r="L25">
+        <v>0.66</v>
+      </c>
+      <c r="M25">
+        <v>0.68</v>
+      </c>
+      <c r="N25">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>30</v>
       </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="b">
-        <v>0</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>25</v>
+      </c>
+      <c r="L27">
+        <v>0.78</v>
+      </c>
+      <c r="M27">
+        <v>0.67</v>
+      </c>
+      <c r="N27">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
         <v>9</v>
       </c>
-      <c r="E21" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="b">
-        <v>0</v>
-      </c>
-      <c r="D22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" t="b">
-        <v>1</v>
-      </c>
-      <c r="G22" t="b">
-        <v>1</v>
-      </c>
-      <c r="H22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>32</v>
       </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="b">
-        <v>0</v>
-      </c>
-      <c r="D23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" t="b">
-        <v>1</v>
-      </c>
-      <c r="G23" t="b">
-        <v>1</v>
-      </c>
-      <c r="H23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>33</v>
       </c>
-      <c r="B25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" t="b">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
         <v>11</v>
       </c>
-      <c r="E25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" t="b">
-        <v>1</v>
-      </c>
-      <c r="G25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H26" t="s">
-        <v>26</v>
+      <c r="E31" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add amazon-walmart base-1 notebooks
</commit_message>
<xml_diff>
--- a/notebooks/amazon-google-results.xlsx
+++ b/notebooks/amazon-google-results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="41040" yWindow="-10740" windowWidth="30900" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="52800" yWindow="-12860" windowWidth="19200" windowHeight="10800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="48">
   <si>
     <t>Vocabulary</t>
   </si>
@@ -110,12 +110,6 @@
     <t>base_2_num</t>
   </si>
   <si>
-    <t>base_1_null</t>
-  </si>
-  <si>
-    <t>base_2_null</t>
-  </si>
-  <si>
     <t>base_1_num_null</t>
   </si>
   <si>
@@ -164,10 +158,16 @@
     <t>Dropout</t>
   </si>
   <si>
-    <t>base_2t_separate</t>
-  </si>
-  <si>
-    <t>Bi-LSTM (not shared)</t>
+    <t>Cosine, Hadamard, Difference</t>
+  </si>
+  <si>
+    <t>Cosine, Inverse_l1, Hadamard, Difference</t>
+  </si>
+  <si>
+    <t>Hadamard, Difference</t>
+  </si>
+  <si>
+    <t>20 / 0.25 / 0.25</t>
   </si>
 </sst>
 </file>
@@ -216,8 +216,54 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -282,7 +328,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="107">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -313,6 +359,29 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -343,6 +412,29 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -618,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -630,7 +722,7 @@
     <col min="2" max="2" width="12.83203125" customWidth="1"/>
     <col min="3" max="3" width="25.33203125" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="27.83203125" customWidth="1"/>
+    <col min="5" max="5" width="37.5" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="21.5" customWidth="1"/>
@@ -656,22 +748,22 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s">
         <v>24</v>
       </c>
       <c r="J1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" t="s">
         <v>35</v>
-      </c>
-      <c r="M1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -758,7 +850,7 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -767,22 +859,22 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J4">
         <v>0.5</v>
       </c>
       <c r="L4">
-        <v>0.73</v>
+        <v>0.89</v>
       </c>
       <c r="M4">
-        <v>0.88</v>
+        <v>0.74</v>
       </c>
       <c r="N4">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -799,7 +891,7 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -807,8 +899,23 @@
       <c r="G5" t="b">
         <v>0</v>
       </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
       <c r="I5" t="s">
-        <v>25</v>
+        <v>40</v>
+      </c>
+      <c r="J5">
+        <v>0.5</v>
+      </c>
+      <c r="L5">
+        <v>0.86</v>
+      </c>
+      <c r="M5">
+        <v>0.82</v>
+      </c>
+      <c r="N5">
+        <v>0.84</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -825,7 +932,7 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -860,7 +967,7 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -868,8 +975,23 @@
       <c r="G8" t="b">
         <v>0</v>
       </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
       <c r="I8" t="s">
-        <v>25</v>
+        <v>40</v>
+      </c>
+      <c r="J8">
+        <v>0.5</v>
+      </c>
+      <c r="L8">
+        <v>0.81</v>
+      </c>
+      <c r="M8">
+        <v>0.74</v>
+      </c>
+      <c r="N8">
+        <v>0.78</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -886,7 +1008,7 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -894,13 +1016,25 @@
       <c r="G9" t="b">
         <v>0</v>
       </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
       <c r="I9" t="s">
-        <v>25</v>
+        <v>40</v>
+      </c>
+      <c r="L9">
+        <v>0.87</v>
+      </c>
+      <c r="M9">
+        <v>0.73</v>
+      </c>
+      <c r="N9">
+        <v>0.79</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -912,7 +1046,7 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -920,8 +1054,23 @@
       <c r="G10" t="b">
         <v>0</v>
       </c>
-      <c r="I10" t="s">
-        <v>25</v>
+      <c r="H10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10">
+        <v>24</v>
+      </c>
+      <c r="J10">
+        <v>0.75</v>
+      </c>
+      <c r="L10">
+        <v>0.83</v>
+      </c>
+      <c r="M10">
+        <v>0.77</v>
+      </c>
+      <c r="N10">
+        <v>0.8</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -973,47 +1122,71 @@
         <v>9</v>
       </c>
       <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13">
+        <v>0.5</v>
+      </c>
+      <c r="L13">
+        <v>0.89</v>
+      </c>
+      <c r="M13">
+        <v>0.76</v>
+      </c>
+      <c r="N13">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
         <v>8</v>
       </c>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" t="s">
-        <v>25</v>
+      <c r="L15">
+        <v>0.83</v>
+      </c>
+      <c r="M15">
+        <v>0.53</v>
+      </c>
+      <c r="N15">
+        <v>0.65</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
@@ -1022,59 +1195,74 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16">
+        <v>0.5</v>
+      </c>
+      <c r="L16">
+        <v>0.85</v>
+      </c>
+      <c r="M16">
+        <v>0.75</v>
+      </c>
+      <c r="N16">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
         <v>7</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E18" t="s">
         <v>8</v>
       </c>
-      <c r="F16" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
         <v>25</v>
       </c>
-      <c r="L16">
-        <v>0.83</v>
-      </c>
-      <c r="M16">
-        <v>0.53</v>
-      </c>
-      <c r="N16">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" t="b">
-        <v>0</v>
-      </c>
-      <c r="D17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" t="b">
-        <v>0</v>
-      </c>
-      <c r="G17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" t="s">
-        <v>25</v>
+      <c r="L18">
+        <v>0.88</v>
+      </c>
+      <c r="M18">
+        <v>0.9</v>
+      </c>
+      <c r="N18">
+        <v>0.89</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -1092,24 +1280,24 @@
         <v>1</v>
       </c>
       <c r="G19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" t="s">
         <v>25</v>
       </c>
       <c r="L19">
-        <v>0.88</v>
+        <v>0.87</v>
       </c>
       <c r="M19">
+        <v>0.92</v>
+      </c>
+      <c r="N19">
         <v>0.9</v>
-      </c>
-      <c r="N19">
-        <v>0.89</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -1121,7 +1309,7 @@
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="F20" t="b">
         <v>1</v>
@@ -1133,54 +1321,54 @@
         <v>25</v>
       </c>
       <c r="L20">
-        <v>0.87</v>
+        <v>0.89</v>
       </c>
       <c r="M20">
-        <v>0.92</v>
+        <v>0.91</v>
       </c>
       <c r="N20">
         <v>0.9</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
+    <row r="21" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
         <v>7</v>
       </c>
-      <c r="E21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" t="b">
-        <v>1</v>
-      </c>
-      <c r="G21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
         <v>25</v>
       </c>
-      <c r="L21">
-        <v>0.89</v>
-      </c>
-      <c r="M21">
-        <v>0.91</v>
-      </c>
-      <c r="N21">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="L22">
+        <v>0.7</v>
+      </c>
+      <c r="M22">
+        <v>0.76</v>
+      </c>
+      <c r="N22">
+        <v>0.73</v>
+      </c>
+    </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
@@ -1189,10 +1377,10 @@
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F23" t="b">
         <v>1</v>
@@ -1200,22 +1388,28 @@
       <c r="G23" t="b">
         <v>0</v>
       </c>
+      <c r="H23" t="s">
+        <v>42</v>
+      </c>
       <c r="I23" t="s">
-        <v>25</v>
+        <v>40</v>
+      </c>
+      <c r="J23">
+        <v>0.5</v>
       </c>
       <c r="L23">
-        <v>0.7</v>
+        <v>0.79</v>
       </c>
       <c r="M23">
-        <v>0.76</v>
+        <v>0.83</v>
       </c>
       <c r="N23">
-        <v>0.73</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
@@ -1224,7 +1418,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
@@ -1233,15 +1427,24 @@
         <v>1</v>
       </c>
       <c r="G24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" t="s">
         <v>25</v>
       </c>
+      <c r="L24">
+        <v>0.78</v>
+      </c>
+      <c r="M24">
+        <v>0.67</v>
+      </c>
+      <c r="N24">
+        <v>0.72</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
@@ -1250,71 +1453,51 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" t="b">
         <v>1</v>
       </c>
+      <c r="H25" t="s">
+        <v>42</v>
+      </c>
       <c r="I25" t="s">
-        <v>25</v>
+        <v>40</v>
+      </c>
+      <c r="J25">
+        <v>0.5</v>
       </c>
       <c r="L25">
-        <v>0.66</v>
+        <v>0.85</v>
       </c>
       <c r="M25">
-        <v>0.68</v>
+        <v>0.83</v>
       </c>
       <c r="N25">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" t="b">
-        <v>0</v>
-      </c>
-      <c r="G26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
       </c>
       <c r="C27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="F27" t="b">
         <v>1</v>
@@ -1322,34 +1505,40 @@
       <c r="G27" t="b">
         <v>1</v>
       </c>
-      <c r="I27" t="s">
-        <v>25</v>
+      <c r="H27" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27">
+        <v>24</v>
+      </c>
+      <c r="J27">
+        <v>0.75</v>
       </c>
       <c r="L27">
-        <v>0.78</v>
+        <v>0.87</v>
       </c>
       <c r="M27">
-        <v>0.67</v>
+        <v>0.82</v>
       </c>
       <c r="N27">
-        <v>0.72</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
@@ -1360,57 +1549,14 @@
       <c r="I28" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" t="b">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" t="s">
-        <v>41</v>
-      </c>
-      <c r="F30" t="b">
-        <v>1</v>
-      </c>
-      <c r="G30" t="b">
-        <v>1</v>
-      </c>
-      <c r="I30" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" t="b">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F31" t="b">
-        <v>1</v>
-      </c>
-      <c r="G31" t="b">
-        <v>1</v>
-      </c>
-      <c r="I31" t="s">
-        <v>25</v>
+      <c r="L28">
+        <v>0.84</v>
+      </c>
+      <c r="M28">
+        <v>0.8</v>
+      </c>
+      <c r="N28">
+        <v>0.82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add spreadsheets of results
</commit_message>
<xml_diff>
--- a/notebooks/amazon-google-results.xlsx
+++ b/notebooks/amazon-google-results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="52800" yWindow="-12860" windowWidth="19200" windowHeight="10800" tabRatio="500"/>
+    <workbookView xWindow="7200" yWindow="5320" windowWidth="19200" windowHeight="10800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -174,7 +174,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -198,6 +198,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -216,7 +221,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="107">
+  <cellStyleXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -324,11 +329,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="107">
+  <cellStyles count="109">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -382,6 +390,7 @@
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -435,6 +444,7 @@
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -712,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="C14" zoomScale="82" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -766,7 +776,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -791,17 +801,17 @@
       <c r="I2" t="s">
         <v>25</v>
       </c>
-      <c r="L2">
-        <v>0.78</v>
-      </c>
-      <c r="M2">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="N2">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L2" s="1">
+        <v>0.77907000000000004</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.57264999999999999</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0.66010000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -826,17 +836,17 @@
       <c r="I3" t="s">
         <v>25</v>
       </c>
-      <c r="L3">
-        <v>0.78</v>
-      </c>
-      <c r="M3">
-        <v>0.68</v>
-      </c>
-      <c r="N3">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L3" s="1">
+        <v>0.78430999999999995</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.68376000000000003</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0.73058999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -867,17 +877,17 @@
       <c r="J4">
         <v>0.5</v>
       </c>
-      <c r="L4">
-        <v>0.89</v>
-      </c>
-      <c r="M4">
-        <v>0.74</v>
-      </c>
-      <c r="N4">
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L4" s="1">
+        <v>0.88775999999999999</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.74358999999999997</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0.80930000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -908,17 +918,17 @@
       <c r="J5">
         <v>0.5</v>
       </c>
-      <c r="L5">
-        <v>0.86</v>
-      </c>
-      <c r="M5">
-        <v>0.82</v>
-      </c>
-      <c r="N5">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L5" s="1">
+        <v>0.85714000000000001</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0.82050999999999996</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0.83843000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -943,17 +953,17 @@
       <c r="I7" t="s">
         <v>25</v>
       </c>
-      <c r="L7">
-        <v>0.79</v>
-      </c>
-      <c r="M7">
-        <v>0.65</v>
-      </c>
-      <c r="N7">
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L7" s="1">
+        <v>0.79166999999999998</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.64956999999999998</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0.71362000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -984,17 +994,17 @@
       <c r="J8">
         <v>0.5</v>
       </c>
-      <c r="L8">
-        <v>0.81</v>
-      </c>
-      <c r="M8">
-        <v>0.74</v>
-      </c>
-      <c r="N8">
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L8" s="1">
+        <v>0.81308000000000002</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0.74358999999999997</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0.77678999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1022,17 +1032,17 @@
       <c r="I9" t="s">
         <v>40</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="1">
         <v>0.87</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="1">
         <v>0.73</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="1">
         <v>0.79</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1063,17 +1073,17 @@
       <c r="J10">
         <v>0.75</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="1">
         <v>0.83</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="1">
         <v>0.77</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="1">
         <v>0.8</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1098,17 +1108,17 @@
       <c r="I12" t="s">
         <v>25</v>
       </c>
-      <c r="L12">
-        <v>0.9</v>
-      </c>
-      <c r="M12">
-        <v>0.84</v>
-      </c>
-      <c r="N12">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L12" s="1">
+        <v>0.89907999999999999</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0.83760999999999997</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0.86726000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1139,17 +1149,17 @@
       <c r="J13">
         <v>0.5</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="1">
         <v>0.89</v>
       </c>
-      <c r="M13">
-        <v>0.76</v>
-      </c>
-      <c r="N13">
-        <v>0.82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M13" s="1">
+        <v>0.76068000000000002</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0.82028000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1174,17 +1184,17 @@
       <c r="I15" t="s">
         <v>25</v>
       </c>
-      <c r="L15">
-        <v>0.83</v>
-      </c>
-      <c r="M15">
-        <v>0.53</v>
-      </c>
-      <c r="N15">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L15" s="1">
+        <v>0.82759000000000005</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0.53332999999999997</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0.64864999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1215,17 +1225,17 @@
       <c r="J16">
         <v>0.5</v>
       </c>
-      <c r="L16">
-        <v>0.85</v>
-      </c>
-      <c r="M16">
-        <v>0.75</v>
-      </c>
-      <c r="N16">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L16" s="1">
+        <v>0.84874000000000005</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0.74814999999999998</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0.79527999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1250,17 +1260,17 @@
       <c r="I18" t="s">
         <v>25</v>
       </c>
-      <c r="L18">
-        <v>0.88</v>
-      </c>
-      <c r="M18">
-        <v>0.9</v>
-      </c>
-      <c r="N18">
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L18" s="1">
+        <v>0.88234999999999997</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0.89744000000000002</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0.88983000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1285,17 +1295,17 @@
       <c r="I19" t="s">
         <v>25</v>
       </c>
-      <c r="L19">
-        <v>0.87</v>
-      </c>
-      <c r="M19">
-        <v>0.92</v>
-      </c>
-      <c r="N19">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L19" s="1">
+        <v>0.87097000000000002</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0.92308000000000001</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0.89627000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1320,18 +1330,18 @@
       <c r="I20" t="s">
         <v>25</v>
       </c>
-      <c r="L20">
-        <v>0.89</v>
-      </c>
-      <c r="M20">
-        <v>0.91</v>
-      </c>
-      <c r="N20">
-        <v>0.9</v>
+      <c r="L20" s="1">
+        <v>0.91891999999999996</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0.87178999999999995</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0.89473999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1356,17 +1366,17 @@
       <c r="I22" t="s">
         <v>25</v>
       </c>
-      <c r="L22">
-        <v>0.7</v>
-      </c>
-      <c r="M22">
-        <v>0.76</v>
-      </c>
-      <c r="N22">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L22" s="1">
+        <v>0.70079000000000002</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0.76068000000000002</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0.72950999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1397,17 +1407,17 @@
       <c r="J23">
         <v>0.5</v>
       </c>
-      <c r="L23">
-        <v>0.79</v>
-      </c>
-      <c r="M23">
-        <v>0.83</v>
-      </c>
-      <c r="N23">
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L23" s="1">
+        <v>0.78861999999999999</v>
+      </c>
+      <c r="M23" s="1">
+        <v>0.82906000000000002</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0.80832999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1432,17 +1442,17 @@
       <c r="I24" t="s">
         <v>25</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="1">
         <v>0.78</v>
       </c>
-      <c r="M24">
-        <v>0.67</v>
-      </c>
-      <c r="N24">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M24" s="1">
+        <v>0.66666999999999998</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0.71889000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1473,17 +1483,17 @@
       <c r="J25">
         <v>0.5</v>
       </c>
-      <c r="L25">
-        <v>0.85</v>
-      </c>
-      <c r="M25">
-        <v>0.83</v>
-      </c>
-      <c r="N25">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L25" s="1">
+        <v>0.85087999999999997</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0.82906000000000002</v>
+      </c>
+      <c r="N25" s="1">
+        <v>0.83982999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1514,17 +1524,17 @@
       <c r="J27">
         <v>0.75</v>
       </c>
-      <c r="L27">
-        <v>0.87</v>
-      </c>
-      <c r="M27">
-        <v>0.82</v>
-      </c>
-      <c r="N27">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L27" s="1">
+        <v>0.87273000000000001</v>
+      </c>
+      <c r="M27" s="1">
+        <v>0.82050999999999996</v>
+      </c>
+      <c r="N27" s="1">
+        <v>0.84580999999999995</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1546,17 +1556,23 @@
       <c r="G28" t="b">
         <v>1</v>
       </c>
-      <c r="I28" t="s">
-        <v>25</v>
-      </c>
-      <c r="L28">
-        <v>0.84</v>
-      </c>
-      <c r="M28">
+      <c r="H28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I28">
+        <v>24</v>
+      </c>
+      <c r="J28">
+        <v>0.75</v>
+      </c>
+      <c r="L28" s="1">
+        <v>0.83721000000000001</v>
+      </c>
+      <c r="M28" s="1">
         <v>0.8</v>
       </c>
-      <c r="N28">
-        <v>0.82</v>
+      <c r="N28" s="1">
+        <v>0.81818000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>